<commit_message>
dads matza cake image
</commit_message>
<xml_diff>
--- a/recipes/recipes.xlsx
+++ b/recipes/recipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\einav\Downloads\einav-yehezkely.github.io\recipes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\einav\clone_here\einav-yehezkely.github.io\recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A057006-640D-41C1-90A8-F3068D4197E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB450EB-0E08-4CFE-A500-D62A89DE238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="21585" windowHeight="12765" xr2:uid="{855B2972-48CC-4AAB-B0C8-66B655037AB0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{855B2972-48CC-4AAB-B0C8-66B655037AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -266,9 +266,6 @@
     <t>קיצ'רי</t>
   </si>
   <si>
-    <t>2 שיני שום|חמאה|&amp;frac12;1 כוס אורז|1 כוס אדשים אדומות|3 כוסות מים|1 רסק עגבניות|פלפל|מלח</t>
-  </si>
-  <si>
     <t>לטגן את שיני השום בחמאה|להוסיף את שאר הדברים</t>
   </si>
   <si>
@@ -345,6 +342,12 @@
   </si>
   <si>
     <t>90 גרם חמאה קוביות|90 גרם אבקת סוכר|105 גרם קמח|90 גרם קורנפלור|1 כפית אבקת אפייה|2 חלמונים</t>
+  </si>
+  <si>
+    <t>/recipes/images/8.jpg</t>
+  </si>
+  <si>
+    <t>2 שיני שום|חמאה|&amp;frac12;1 כוס אורז|1 כוס עדשים אדומות|3 כוסות מים|1 רסק עגבניות|פלפל|מלח</t>
   </si>
 </sst>
 </file>
@@ -734,7 +737,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -804,10 +807,10 @@
         <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>72</v>
@@ -830,13 +833,13 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -844,25 +847,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -873,7 +876,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>32</v>
@@ -916,7 +919,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -936,22 +939,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -981,6 +984,9 @@
       <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1036,25 +1042,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -1170,16 +1176,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>